<commit_message>
working flow for generating wbs tasks in the xlsx file and upload to SP
</commit_message>
<xml_diff>
--- a/ai_app/wbs.xlsx
+++ b/ai_app/wbs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecfdata.sharepoint.com/sites/ECF-POM/Shared Documents/Templates/Hours Estimates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ecfdata-my.sharepoint.com/personal/talha_jaleel_ecfdata_com/Documents/Desktop/ECf Sales AI enablement/Code/Backend/ECFSalesAI/ai_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="299" documentId="8_{00E8CCA3-022B-4FB1-958B-9762B3311849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95220F03-C89A-49CA-AD67-AB3A8842EE8B}"/>
+  <xr:revisionPtr revIDLastSave="301" documentId="8_{00E8CCA3-022B-4FB1-958B-9762B3311849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{516788D8-A3CF-4500-A305-F8F4058F30EA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{38A6DC79-F9FB-45AA-88DD-B25A2C2713A8}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13749" firstSheet="1" activeTab="3" xr2:uid="{38A6DC79-F9FB-45AA-88DD-B25A2C2713A8}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="4" r:id="rId1"/>
@@ -720,7 +720,7 @@
     <numFmt numFmtId="164" formatCode="0.0\ &quot;Hrs&quot;"/>
     <numFmt numFmtId="165" formatCode="0.00\ &quot;Hrs&quot;"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1822,13 +1822,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1866,9 +1866,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1906,7 +1906,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2012,7 +2012,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2154,7 +2154,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2197,19 +2197,19 @@
       <selection activeCell="B3" activeCellId="1" sqref="B2 B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" style="41" customWidth="1"/>
+    <col min="1" max="1" width="5.69140625" style="41" customWidth="1"/>
     <col min="2" max="2" width="142" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375"/>
-    <col min="5" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.69140625" customWidth="1"/>
+    <col min="4" max="4" width="8.69140625"/>
+    <col min="5" max="6" width="12.69140625" customWidth="1"/>
+    <col min="7" max="7" width="5.69140625" customWidth="1"/>
+    <col min="8" max="8" width="10.84375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="18.75">
+    <row r="2" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A2" s="140">
         <v>1</v>
       </c>
@@ -2224,7 +2224,7 @@
       <c r="H2" s="35"/>
       <c r="I2" s="36"/>
     </row>
-    <row r="3" spans="1:9" ht="18.75">
+    <row r="3" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A3" s="140"/>
       <c r="B3" s="124" t="s">
         <v>1</v>
@@ -2237,7 +2237,7 @@
       <c r="H3" s="35"/>
       <c r="I3" s="36"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75">
+    <row r="4" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A4" s="140"/>
       <c r="B4" s="124" t="s">
         <v>2</v>
@@ -2250,7 +2250,7 @@
       <c r="H4" s="36"/>
       <c r="I4" s="35"/>
     </row>
-    <row r="5" spans="1:9" ht="18.75">
+    <row r="5" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A5" s="40"/>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -2260,7 +2260,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="18.75">
+    <row r="6" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A6" s="140">
         <v>2</v>
       </c>
@@ -2274,7 +2274,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="18.75">
+    <row r="7" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A7" s="140"/>
       <c r="B7" s="33" t="s">
         <v>4</v>
@@ -2286,7 +2286,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="42.75" customHeight="1">
+    <row r="8" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="140"/>
       <c r="B8" s="50" t="s">
         <v>5</v>
@@ -2298,7 +2298,7 @@
       <c r="G8" s="4"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="18.75">
+    <row r="9" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="B9" s="1"/>
       <c r="C9" s="33"/>
       <c r="D9" s="4"/>
@@ -2307,7 +2307,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="18.75">
+    <row r="10" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A10" s="140">
         <v>3</v>
       </c>
@@ -2321,30 +2321,30 @@
       <c r="G10" s="4"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="18.75">
+    <row r="11" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A11" s="140"/>
       <c r="B11" s="33" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="33"/>
     </row>
-    <row r="12" spans="1:9" ht="18.75">
+    <row r="12" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A12" s="140"/>
       <c r="B12" s="33" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18.75">
+    <row r="13" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A13" s="140"/>
       <c r="B13" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="38"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="C14" s="38"/>
     </row>
-    <row r="15" spans="1:9" ht="18.75">
+    <row r="15" spans="1:9" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A15" s="140">
         <v>4</v>
       </c>
@@ -2352,22 +2352,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="37.5">
+    <row r="16" spans="1:9" ht="36.9" x14ac:dyDescent="0.5">
       <c r="A16" s="140"/>
       <c r="B16" s="62" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.75">
+    <row r="17" spans="1:2" ht="18.45" x14ac:dyDescent="0.4">
       <c r="A17" s="140"/>
       <c r="B17" s="57" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.75">
+    <row r="18" spans="1:2" ht="18.45" x14ac:dyDescent="0.4">
       <c r="B18" s="57"/>
     </row>
-    <row r="20" spans="1:2" ht="75">
+    <row r="20" spans="1:2" ht="55.3" x14ac:dyDescent="0.4">
       <c r="A20" s="39">
         <v>5</v>
       </c>
@@ -2403,44 +2403,44 @@
       <selection activeCell="K11" sqref="K11:N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.53515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="34" style="4" customWidth="1"/>
-    <col min="4" max="5" width="12.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="4" customWidth="1"/>
-    <col min="7" max="8" width="8.7109375" style="4"/>
-    <col min="9" max="9" width="5.7109375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="79.7109375" style="9" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="4"/>
-    <col min="13" max="14" width="12.7109375" style="4" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.69140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="5.69140625" style="4" customWidth="1"/>
+    <col min="7" max="8" width="8.69140625" style="4"/>
+    <col min="9" max="9" width="5.69140625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.69140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="79.69140625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="8.69140625" style="4"/>
+    <col min="13" max="14" width="12.69140625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="5.69140625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12.3828125" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" style="3" customWidth="1"/>
-    <col min="18" max="18" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" style="4"/>
-    <col min="20" max="21" width="12.7109375" style="4" customWidth="1"/>
-    <col min="22" max="22" width="5.7109375" style="4" customWidth="1"/>
-    <col min="23" max="23" width="8.7109375" style="4"/>
-    <col min="24" max="24" width="5.7109375" style="4" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="3" customWidth="1"/>
-    <col min="26" max="26" width="75.7109375" style="4" customWidth="1"/>
-    <col min="27" max="27" width="8.7109375" style="4"/>
-    <col min="28" max="29" width="12.7109375" style="4" customWidth="1"/>
-    <col min="30" max="30" width="5.7109375" style="4" customWidth="1"/>
-    <col min="31" max="31" width="8.7109375" style="4"/>
-    <col min="32" max="32" width="5.7109375" style="4" customWidth="1"/>
-    <col min="33" max="33" width="12.7109375" style="3" customWidth="1"/>
-    <col min="34" max="34" width="75.7109375" style="4" customWidth="1"/>
-    <col min="35" max="35" width="8.7109375" style="4"/>
-    <col min="36" max="37" width="12.7109375" style="4" customWidth="1"/>
-    <col min="38" max="38" width="5.7109375" style="4" customWidth="1"/>
-    <col min="39" max="16384" width="8.7109375" style="4"/>
+    <col min="18" max="18" width="6.3828125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.69140625" style="4"/>
+    <col min="20" max="21" width="12.69140625" style="4" customWidth="1"/>
+    <col min="22" max="22" width="5.69140625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="8.69140625" style="4"/>
+    <col min="24" max="24" width="5.69140625" style="4" customWidth="1"/>
+    <col min="25" max="25" width="12.69140625" style="3" customWidth="1"/>
+    <col min="26" max="26" width="75.69140625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="8.69140625" style="4"/>
+    <col min="28" max="29" width="12.69140625" style="4" customWidth="1"/>
+    <col min="30" max="30" width="5.69140625" style="4" customWidth="1"/>
+    <col min="31" max="31" width="8.69140625" style="4"/>
+    <col min="32" max="32" width="5.69140625" style="4" customWidth="1"/>
+    <col min="33" max="33" width="12.69140625" style="3" customWidth="1"/>
+    <col min="34" max="34" width="75.69140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="8.69140625" style="4"/>
+    <col min="36" max="37" width="12.69140625" style="4" customWidth="1"/>
+    <col min="38" max="38" width="5.69140625" style="4" customWidth="1"/>
+    <col min="39" max="16384" width="8.69140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="84" customFormat="1" ht="25.5">
+    <row r="1" spans="1:33" s="84" customFormat="1" ht="23.15" x14ac:dyDescent="0.4">
       <c r="A1" s="82" t="s">
         <v>14</v>
       </c>
@@ -2466,7 +2466,7 @@
       <c r="Y1" s="85"/>
       <c r="AG1" s="85"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
@@ -2489,7 +2489,7 @@
       <c r="Y2" s="4"/>
       <c r="AG2" s="4"/>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A3" s="18"/>
       <c r="B3" s="6"/>
       <c r="C3" s="5"/>
@@ -2511,7 +2511,7 @@
       <c r="Y3" s="4"/>
       <c r="AG3" s="4"/>
     </row>
-    <row r="4" spans="1:33" ht="18.95" customHeight="1">
+    <row r="4" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="20"/>
       <c r="B4" s="3" t="s">
         <v>19</v>
@@ -2539,7 +2539,7 @@
       <c r="Y4" s="4"/>
       <c r="AG4" s="4"/>
     </row>
-    <row r="5" spans="1:33" ht="18">
+    <row r="5" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A5" s="20"/>
       <c r="B5" s="3" t="s">
         <v>21</v>
@@ -2561,7 +2561,7 @@
       <c r="Y5" s="4"/>
       <c r="AG5" s="4"/>
     </row>
-    <row r="6" spans="1:33" ht="18">
+    <row r="6" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A6" s="20"/>
       <c r="B6" s="3" t="s">
         <v>23</v>
@@ -2583,7 +2583,7 @@
       <c r="Y6" s="4"/>
       <c r="AG6" s="4"/>
     </row>
-    <row r="7" spans="1:33" ht="18">
+    <row r="7" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A7" s="20"/>
       <c r="B7" s="3" t="s">
         <v>25</v>
@@ -2603,7 +2603,7 @@
       <c r="Y7" s="4"/>
       <c r="AG7" s="4"/>
     </row>
-    <row r="8" spans="1:33" ht="18.75" thickBot="1">
+    <row r="8" spans="1:33" ht="18.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="20"/>
       <c r="B8" s="96" t="s">
         <v>26</v>
@@ -2623,7 +2623,7 @@
       <c r="Y8" s="4"/>
       <c r="AG8" s="4"/>
     </row>
-    <row r="9" spans="1:33" ht="18">
+    <row r="9" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A9" s="20"/>
       <c r="B9" s="8" t="s">
         <v>27</v>
@@ -2642,7 +2642,7 @@
       <c r="Y9" s="4"/>
       <c r="AG9" s="4"/>
     </row>
-    <row r="10" spans="1:33" ht="18" thickBot="1">
+    <row r="10" spans="1:33" ht="18.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="23"/>
       <c r="B10" s="24"/>
       <c r="C10" s="25"/>
@@ -2665,7 +2665,7 @@
       <c r="Y10" s="4"/>
       <c r="AG10" s="4"/>
     </row>
-    <row r="11" spans="1:33" ht="18">
+    <row r="11" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="B11" s="8"/>
       <c r="D11" s="2"/>
       <c r="E11" s="11"/>
@@ -2677,7 +2677,7 @@
       <c r="Y11" s="4"/>
       <c r="AG11" s="4"/>
     </row>
-    <row r="12" spans="1:33" ht="33.75">
+    <row r="12" spans="1:33" ht="33.450000000000003" x14ac:dyDescent="0.4">
       <c r="A12" s="148" t="s">
         <v>30</v>
       </c>
@@ -2692,7 +2692,7 @@
       <c r="Y12" s="4"/>
       <c r="AG12" s="4"/>
     </row>
-    <row r="13" spans="1:33" ht="18.75" thickBot="1">
+    <row r="13" spans="1:33" ht="18.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B13" s="4"/>
       <c r="K13" s="91"/>
       <c r="L13" s="44"/>
@@ -2702,7 +2702,7 @@
       <c r="Y13" s="4"/>
       <c r="AG13" s="4"/>
     </row>
-    <row r="14" spans="1:33" ht="18">
+    <row r="14" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="B14" s="149" t="s">
         <v>31</v>
       </c>
@@ -2723,7 +2723,7 @@
       <c r="Y14" s="4"/>
       <c r="AG14" s="4"/>
     </row>
-    <row r="15" spans="1:33" ht="18">
+    <row r="15" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="B15" s="151" t="s">
         <v>32</v>
       </c>
@@ -2743,7 +2743,7 @@
       <c r="Y15" s="4"/>
       <c r="AG15" s="4"/>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A16" s="29"/>
       <c r="B16" s="151" t="s">
         <v>33</v>
@@ -2773,7 +2773,7 @@
       <c r="Y16" s="4"/>
       <c r="AG16" s="4"/>
     </row>
-    <row r="17" spans="1:33" ht="18">
+    <row r="17" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A17" s="30"/>
       <c r="B17" s="153" t="s">
         <v>35</v>
@@ -2796,7 +2796,7 @@
       <c r="Y17" s="4"/>
       <c r="AG17" s="4"/>
     </row>
-    <row r="18" spans="1:33" ht="18.75" thickBot="1">
+    <row r="18" spans="1:33" ht="18.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="143" t="s">
         <v>36</v>
@@ -2820,7 +2820,7 @@
       <c r="Y18" s="4"/>
       <c r="AG18" s="4"/>
     </row>
-    <row r="19" spans="1:33" ht="21.95" customHeight="1" thickBot="1">
+    <row r="19" spans="1:33" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
       <c r="B19" s="145" t="s">
         <v>37</v>
@@ -2843,7 +2843,7 @@
       <c r="Y19" s="4"/>
       <c r="AG19" s="4"/>
     </row>
-    <row r="20" spans="1:33" ht="23.25" customHeight="1">
+    <row r="20" spans="1:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="2"/>
@@ -2865,7 +2865,7 @@
       <c r="Y20" s="4"/>
       <c r="AG20" s="4"/>
     </row>
-    <row r="21" spans="1:33" ht="18">
+    <row r="21" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="75" t="s">
         <v>39</v>
@@ -2882,7 +2882,7 @@
       <c r="Y21" s="4"/>
       <c r="AG21" s="4"/>
     </row>
-    <row r="22" spans="1:33" ht="18">
+    <row r="22" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="75" t="s">
         <v>40</v>
@@ -2899,7 +2899,7 @@
       <c r="Y22" s="4"/>
       <c r="AG22" s="4"/>
     </row>
-    <row r="23" spans="1:33" ht="18.75" thickBot="1">
+    <row r="23" spans="1:33" ht="18.45" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
       <c r="B23" s="78" t="s">
         <v>41</v>
@@ -2919,7 +2919,7 @@
       <c r="Y23" s="4"/>
       <c r="AG23" s="4"/>
     </row>
-    <row r="24" spans="1:33" ht="18.95" customHeight="1">
+    <row r="24" spans="1:33" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B24" s="4"/>
       <c r="C24" s="77"/>
       <c r="E24" s="2"/>
@@ -2934,7 +2934,7 @@
       <c r="Y24" s="4"/>
       <c r="AG24" s="4"/>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="B25" s="4"/>
       <c r="C25" s="73"/>
       <c r="E25" s="2"/>
@@ -2943,7 +2943,7 @@
       <c r="Y25" s="4"/>
       <c r="AG25" s="4"/>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="B26" s="4"/>
       <c r="C26" s="138"/>
       <c r="E26" s="2"/>
@@ -2951,186 +2951,186 @@
       <c r="Y26" s="4"/>
       <c r="AG26" s="4"/>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="C27" s="139"/>
       <c r="E27" s="2"/>
       <c r="X27" s="3"/>
       <c r="Y27" s="4"/>
       <c r="AG27" s="4"/>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="C28" s="139"/>
       <c r="E28" s="2"/>
       <c r="X28" s="3"/>
       <c r="Y28" s="4"/>
       <c r="AG28" s="4"/>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="C29" s="139"/>
       <c r="E29" s="2"/>
       <c r="X29" s="3"/>
       <c r="Y29" s="4"/>
       <c r="AG29" s="4"/>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E30" s="2"/>
       <c r="X30" s="3"/>
       <c r="Y30" s="4"/>
       <c r="AG30" s="4"/>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E31" s="2"/>
       <c r="X31" s="3"/>
       <c r="Y31" s="4"/>
       <c r="AG31" s="4"/>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E32" s="2"/>
       <c r="X32" s="3"/>
       <c r="Y32" s="4"/>
       <c r="AG32" s="4"/>
     </row>
-    <row r="33" spans="5:33">
+    <row r="33" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E33" s="2"/>
       <c r="X33" s="3"/>
       <c r="Y33" s="4"/>
       <c r="AG33" s="4"/>
     </row>
-    <row r="34" spans="5:33">
+    <row r="34" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E34" s="2"/>
       <c r="X34" s="3"/>
       <c r="Y34" s="4"/>
       <c r="AG34" s="4"/>
     </row>
-    <row r="35" spans="5:33" ht="18.95" customHeight="1">
+    <row r="35" spans="5:33" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E35" s="2"/>
       <c r="X35" s="3"/>
       <c r="Y35" s="4"/>
       <c r="AG35" s="4"/>
     </row>
-    <row r="36" spans="5:33">
+    <row r="36" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E36" s="2"/>
       <c r="X36" s="3"/>
       <c r="Y36" s="4"/>
       <c r="AG36" s="4"/>
     </row>
-    <row r="37" spans="5:33">
+    <row r="37" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E37" s="2"/>
       <c r="X37" s="3"/>
       <c r="Y37" s="4"/>
       <c r="AG37" s="4"/>
     </row>
-    <row r="38" spans="5:33">
+    <row r="38" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E38" s="2"/>
       <c r="X38" s="3"/>
       <c r="Y38" s="4"/>
       <c r="AG38" s="4"/>
     </row>
-    <row r="39" spans="5:33">
+    <row r="39" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E39" s="2"/>
       <c r="X39" s="3"/>
       <c r="Y39" s="4"/>
       <c r="AG39" s="4"/>
     </row>
-    <row r="40" spans="5:33">
+    <row r="40" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E40" s="2"/>
       <c r="X40" s="3"/>
       <c r="Y40" s="4"/>
       <c r="AG40" s="4"/>
     </row>
-    <row r="41" spans="5:33">
+    <row r="41" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E41" s="2"/>
       <c r="X41" s="3"/>
       <c r="Y41" s="4"/>
       <c r="AG41" s="4"/>
     </row>
-    <row r="42" spans="5:33">
+    <row r="42" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E42" s="2"/>
       <c r="X42" s="3"/>
       <c r="Y42" s="4"/>
       <c r="AG42" s="4"/>
     </row>
-    <row r="43" spans="5:33">
+    <row r="43" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E43" s="2"/>
       <c r="X43" s="3"/>
       <c r="Y43" s="4"/>
       <c r="AG43" s="4"/>
     </row>
-    <row r="44" spans="5:33" ht="18.95" customHeight="1">
+    <row r="44" spans="5:33" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="E44" s="2"/>
       <c r="X44" s="3"/>
       <c r="Y44" s="4"/>
       <c r="AG44" s="4"/>
     </row>
-    <row r="45" spans="5:33">
+    <row r="45" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E45" s="2"/>
       <c r="X45" s="3"/>
       <c r="Y45" s="4"/>
       <c r="AG45" s="4"/>
     </row>
-    <row r="46" spans="5:33">
+    <row r="46" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E46" s="2"/>
       <c r="X46" s="3"/>
       <c r="Y46" s="4"/>
       <c r="AG46" s="4"/>
     </row>
-    <row r="47" spans="5:33">
+    <row r="47" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E47" s="2"/>
       <c r="X47" s="3"/>
       <c r="Y47" s="4"/>
       <c r="AG47" s="4"/>
     </row>
-    <row r="48" spans="5:33">
+    <row r="48" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E48" s="2"/>
       <c r="X48" s="3"/>
       <c r="Y48" s="4"/>
       <c r="AG48" s="4"/>
     </row>
-    <row r="49" spans="5:33">
+    <row r="49" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E49" s="2"/>
       <c r="X49" s="3"/>
       <c r="Y49" s="4"/>
       <c r="AG49" s="4"/>
     </row>
-    <row r="50" spans="5:33">
+    <row r="50" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E50" s="2"/>
       <c r="X50" s="3"/>
       <c r="Y50" s="4"/>
       <c r="AG50" s="4"/>
     </row>
-    <row r="51" spans="5:33">
+    <row r="51" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="E51" s="2"/>
       <c r="X51" s="3"/>
       <c r="Y51" s="4"/>
       <c r="AG51" s="4"/>
     </row>
-    <row r="52" spans="5:33">
+    <row r="52" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="X52" s="3"/>
       <c r="Y52" s="4"/>
       <c r="AG52" s="4"/>
     </row>
-    <row r="53" spans="5:33">
+    <row r="53" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="X53" s="3"/>
       <c r="Y53" s="4"/>
       <c r="AG53" s="4"/>
     </row>
-    <row r="54" spans="5:33">
+    <row r="54" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="X54" s="3"/>
       <c r="Y54" s="4"/>
       <c r="AG54" s="4"/>
     </row>
-    <row r="55" spans="5:33">
+    <row r="55" spans="5:33" ht="18" x14ac:dyDescent="0.4">
       <c r="X55" s="3"/>
       <c r="Y55" s="4"/>
       <c r="AG55" s="4"/>
     </row>
-    <row r="56" spans="5:33"/>
-    <row r="57" spans="5:33"/>
-    <row r="59" spans="5:33"/>
-    <row r="62" spans="5:33"/>
-    <row r="63" spans="5:33"/>
-    <row r="64" spans="5:33"/>
-    <row r="65"/>
+    <row r="56" spans="5:33" ht="18" x14ac:dyDescent="0.4"/>
+    <row r="57" spans="5:33" ht="18" x14ac:dyDescent="0.4"/>
+    <row r="59" spans="5:33" ht="18" x14ac:dyDescent="0.4"/>
+    <row r="62" spans="5:33" ht="18" x14ac:dyDescent="0.4"/>
+    <row r="63" spans="5:33" ht="18" x14ac:dyDescent="0.4"/>
+    <row r="64" spans="5:33" ht="18" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="18" x14ac:dyDescent="0.4"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="GViGtwF82774P+JgvBvfgkGMhIrFhpl6LyEjg+Vkp5UpPKPM6S7UU12oMBnnUzqSQtdCEnnj4sAHP+DRXP1K9w==" saltValue="CZfnMMHsjuDGDgkOR9NE2A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
@@ -3164,18 +3164,18 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="68.5703125" customWidth="1"/>
-    <col min="11" max="11" width="55.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.15234375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="68.53515625" customWidth="1"/>
+    <col min="11" max="11" width="55.3828125" customWidth="1"/>
+    <col min="12" max="12" width="18.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.25">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.45">
       <c r="C1" s="51" t="s">
         <v>44</v>
       </c>
@@ -3186,7 +3186,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18.75">
+    <row r="2" spans="1:16" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A2" s="51" t="s">
         <v>47</v>
       </c>
@@ -3208,7 +3208,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18">
+    <row r="3" spans="1:16" ht="16.75" x14ac:dyDescent="0.5">
       <c r="A3" s="74" t="s">
         <v>52</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="18">
+    <row r="4" spans="1:16" ht="16.75" x14ac:dyDescent="0.5">
       <c r="A4" s="74" t="s">
         <v>61</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="18">
+    <row r="5" spans="1:16" ht="16.75" x14ac:dyDescent="0.5">
       <c r="A5" s="74" t="s">
         <v>65</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="18">
+    <row r="6" spans="1:16" ht="16.75" x14ac:dyDescent="0.5">
       <c r="A6" s="74" t="s">
         <v>71</v>
       </c>
@@ -3339,7 +3339,7 @@
       <c r="O6" s="88"/>
       <c r="P6" s="88"/>
     </row>
-    <row r="7" spans="1:16" ht="18">
+    <row r="7" spans="1:16" ht="16.75" x14ac:dyDescent="0.5">
       <c r="A7" s="74" t="s">
         <v>75</v>
       </c>
@@ -3363,7 +3363,7 @@
       <c r="O7" s="88"/>
       <c r="P7" s="88"/>
     </row>
-    <row r="8" spans="1:16" ht="18">
+    <row r="8" spans="1:16" ht="16.75" x14ac:dyDescent="0.5">
       <c r="A8" s="74" t="s">
         <v>80</v>
       </c>
@@ -3388,7 +3388,7 @@
       <c r="O8" s="88"/>
       <c r="P8" s="88"/>
     </row>
-    <row r="9" spans="1:16" ht="18">
+    <row r="9" spans="1:16" ht="16.75" x14ac:dyDescent="0.5">
       <c r="A9" s="74" t="s">
         <v>85</v>
       </c>
@@ -3409,7 +3409,7 @@
       <c r="O9" s="88"/>
       <c r="P9" s="88"/>
     </row>
-    <row r="10" spans="1:16" ht="18">
+    <row r="10" spans="1:16" ht="16.75" x14ac:dyDescent="0.5">
       <c r="B10" s="52" t="s">
         <v>87</v>
       </c>
@@ -3429,7 +3429,7 @@
       <c r="O10" s="88"/>
       <c r="P10" s="88"/>
     </row>
-    <row r="11" spans="1:16" ht="18">
+    <row r="11" spans="1:16" ht="16.75" x14ac:dyDescent="0.5">
       <c r="E11" t="s">
         <v>90</v>
       </c>
@@ -3445,7 +3445,7 @@
       <c r="O11" s="88"/>
       <c r="P11" s="88"/>
     </row>
-    <row r="13" spans="1:16" ht="15.75">
+    <row r="13" spans="1:16" ht="15.9" x14ac:dyDescent="0.45">
       <c r="C13" s="51" t="s">
         <v>44</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15.75">
+    <row r="14" spans="1:16" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A14" s="51" t="s">
         <v>20</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A15" s="74" t="s">
         <v>95</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A16" s="74" t="s">
         <v>97</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" s="74" t="s">
         <v>75</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" s="74" t="s">
         <v>99</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="74" t="s">
         <v>85</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="74" t="s">
         <v>80</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="74" t="s">
         <v>105</v>
       </c>
@@ -3589,7 +3589,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75">
+    <row r="22" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
       <c r="B22" s="53" t="s">
         <v>87</v>
       </c>
@@ -3598,12 +3598,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75">
+    <row r="25" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
       <c r="C25" s="51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75">
+    <row r="26" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A26" s="51" t="s">
         <v>28</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="74" t="s">
         <v>75</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="74" t="s">
         <v>99</v>
       </c>
@@ -3634,7 +3634,7 @@
       </c>
       <c r="C28" s="55"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="74" t="s">
         <v>85</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="74"/>
       <c r="B30" t="s">
         <v>103</v>
@@ -3656,7 +3656,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="74" t="s">
         <v>105</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75">
+    <row r="32" spans="1:6" ht="15.9" x14ac:dyDescent="0.45">
       <c r="B32" s="53" t="s">
         <v>87</v>
       </c>
@@ -3677,12 +3677,12 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75">
+    <row r="35" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="C35" s="51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75">
+    <row r="36" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A36" s="51" t="s">
         <v>34</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="74" t="s">
         <v>75</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" s="74" t="s">
         <v>99</v>
       </c>
@@ -3713,7 +3713,7 @@
       </c>
       <c r="C38" s="55"/>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" s="74" t="s">
         <v>85</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" s="74"/>
       <c r="B40" t="s">
         <v>103</v>
@@ -3735,7 +3735,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" s="74" t="s">
         <v>105</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75">
+    <row r="42" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="B42" s="53" t="s">
         <v>87</v>
       </c>
@@ -3756,12 +3756,12 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75">
+    <row r="45" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="C45" s="51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75">
+    <row r="46" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="A46" s="51" t="s">
         <v>38</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A47" s="74" t="s">
         <v>75</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" s="74" t="s">
         <v>99</v>
       </c>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="C48" s="55"/>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49" s="74" t="s">
         <v>85</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A50" s="74"/>
       <c r="B50" t="s">
         <v>103</v>
@@ -3814,7 +3814,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" customHeight="1">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="74" t="s">
         <v>105</v>
       </c>
@@ -3826,7 +3826,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1">
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B52" s="53" t="s">
         <v>87</v>
       </c>
@@ -3835,16 +3835,16 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1">
+    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B53" s="52"/>
       <c r="C53" s="59"/>
     </row>
-    <row r="55" spans="1:3" ht="15.75">
+    <row r="55" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="C55" s="51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="31.5">
+    <row r="56" spans="1:3" ht="31.75" x14ac:dyDescent="0.45">
       <c r="A56" s="58" t="s">
         <v>107</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A57" s="74" t="s">
         <v>75</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A58" s="74" t="s">
         <v>99</v>
       </c>
@@ -3875,7 +3875,7 @@
       </c>
       <c r="C58" s="55"/>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A59" s="74" t="s">
         <v>108</v>
       </c>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="C59" s="55"/>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A60" s="74" t="s">
         <v>110</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A61" s="74" t="s">
         <v>112</v>
       </c>
@@ -3904,7 +3904,7 @@
       </c>
       <c r="C61" s="55"/>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A62" s="74" t="s">
         <v>85</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A63" s="74"/>
       <c r="B63" t="s">
         <v>103</v>
@@ -3926,7 +3926,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A64" s="74" t="s">
         <v>105</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="2:3" ht="15.75">
+    <row r="65" spans="2:3" ht="15.9" x14ac:dyDescent="0.45">
       <c r="B65" s="53" t="s">
         <v>87</v>
       </c>
@@ -3964,31 +3964,31 @@
       <selection pane="bottomLeft" activeCell="A15" sqref="A15:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="16.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="117" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="117" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="119" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.7109375" style="132" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="118" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" style="117" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="117" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="119" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.7109375" style="132" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" style="118" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" style="117" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" style="117" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="119" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="60.7109375" style="132" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" style="118" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="117" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" style="117" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="119" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="60.7109375" style="132" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="119"/>
+    <col min="1" max="1" width="6.15234375" style="117" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3828125" style="117" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.3046875" style="119" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.69140625" style="132" customWidth="1"/>
+    <col min="5" max="5" width="5.69140625" style="118" customWidth="1"/>
+    <col min="6" max="6" width="6.15234375" style="117" customWidth="1"/>
+    <col min="7" max="7" width="9.3828125" style="117" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.15234375" style="119" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.69140625" style="132" customWidth="1"/>
+    <col min="10" max="10" width="5.69140625" style="118" customWidth="1"/>
+    <col min="11" max="11" width="6.15234375" style="117" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.3828125" style="117" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.15234375" style="119" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.69140625" style="132" customWidth="1"/>
+    <col min="15" max="15" width="5.53515625" style="118" customWidth="1"/>
+    <col min="16" max="16" width="6.15234375" style="117" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.3828125" style="117" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.15234375" style="119" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="60.69140625" style="132" customWidth="1"/>
+    <col min="20" max="16384" width="9.15234375" style="119"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18.75">
+    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.5">
       <c r="A1" s="113" t="s">
         <v>115</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="18.75">
+    <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.5">
       <c r="A2" s="115"/>
       <c r="B2" s="116"/>
       <c r="C2" s="116"/>
@@ -4056,7 +4056,7 @@
       <c r="R2" s="116"/>
       <c r="S2" s="135"/>
     </row>
-    <row r="3" spans="1:19" ht="23.25">
+    <row r="3" spans="1:19" ht="23.6" x14ac:dyDescent="0.5">
       <c r="A3" s="103" t="s">
         <v>118</v>
       </c>
@@ -4111,34 +4111,34 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="23.25" customHeight="1">
-      <c r="A4" s="155" t="s">
+    <row r="4" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="157" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="155"/>
-      <c r="C4" s="155"/>
-      <c r="D4" s="155"/>
+      <c r="B4" s="157"/>
+      <c r="C4" s="157"/>
+      <c r="D4" s="157"/>
       <c r="E4" s="121"/>
-      <c r="F4" s="155" t="s">
+      <c r="F4" s="157" t="s">
         <v>123</v>
       </c>
-      <c r="G4" s="155"/>
-      <c r="H4" s="155"/>
-      <c r="I4" s="155"/>
-      <c r="K4" s="155" t="s">
+      <c r="G4" s="157"/>
+      <c r="H4" s="157"/>
+      <c r="I4" s="157"/>
+      <c r="K4" s="157" t="s">
         <v>123</v>
       </c>
-      <c r="L4" s="155"/>
-      <c r="M4" s="155"/>
-      <c r="N4" s="155"/>
-      <c r="P4" s="155" t="s">
+      <c r="L4" s="157"/>
+      <c r="M4" s="157"/>
+      <c r="N4" s="157"/>
+      <c r="P4" s="157" t="s">
         <v>123</v>
       </c>
-      <c r="Q4" s="155"/>
-      <c r="R4" s="155"/>
-      <c r="S4" s="155"/>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="Q4" s="157"/>
+      <c r="R4" s="157"/>
+      <c r="S4" s="157"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A5" s="102"/>
       <c r="B5" s="102" t="s">
         <v>118</v>
@@ -4176,7 +4176,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A6" s="102" t="s">
         <v>118</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="18" customHeight="1">
+    <row r="7" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="102"/>
       <c r="B7" s="102" t="s">
         <v>118</v>
@@ -4251,7 +4251,7 @@
       <c r="R7" s="156"/>
       <c r="S7" s="156"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A8" s="102"/>
       <c r="B8" s="102" t="s">
         <v>118</v>
@@ -4282,13 +4282,13 @@
       <c r="R8" s="156"/>
       <c r="S8" s="156"/>
     </row>
-    <row r="9" spans="1:19" s="128" customFormat="1">
-      <c r="A9" s="157" t="s">
+    <row r="9" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="155" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="157"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
+      <c r="B9" s="155"/>
+      <c r="C9" s="155"/>
+      <c r="D9" s="155"/>
       <c r="E9" s="125"/>
       <c r="F9" s="126" t="s">
         <v>118</v>
@@ -4329,13 +4329,13 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="128" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A10" s="157" t="s">
+    <row r="10" spans="1:19" s="128" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="155" t="s">
         <v>131</v>
       </c>
-      <c r="B10" s="157"/>
-      <c r="C10" s="157"/>
-      <c r="D10" s="157"/>
+      <c r="B10" s="155"/>
+      <c r="C10" s="155"/>
+      <c r="D10" s="155"/>
       <c r="E10" s="125"/>
       <c r="F10" s="126"/>
       <c r="G10" s="126"/>
@@ -4360,7 +4360,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="128" customFormat="1">
+    <row r="11" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A11" s="126" t="s">
         <v>118</v>
       </c>
@@ -4399,7 +4399,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="128" customFormat="1" ht="21.75" customHeight="1">
+    <row r="12" spans="1:19" s="128" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="126"/>
       <c r="B12" s="126"/>
       <c r="C12" s="127">
@@ -4424,7 +4424,7 @@
       <c r="R12" s="127"/>
       <c r="S12" s="131"/>
     </row>
-    <row r="13" spans="1:19" s="128" customFormat="1">
+    <row r="13" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A13" s="126"/>
       <c r="B13" s="126"/>
       <c r="C13" s="127"/>
@@ -4447,7 +4447,7 @@
       <c r="R13" s="127"/>
       <c r="S13" s="131"/>
     </row>
-    <row r="14" spans="1:19" s="128" customFormat="1">
+    <row r="14" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="126"/>
       <c r="B14" s="126"/>
       <c r="C14" s="127"/>
@@ -4468,7 +4468,7 @@
       <c r="R14" s="127"/>
       <c r="S14" s="131"/>
     </row>
-    <row r="15" spans="1:19" s="128" customFormat="1">
+    <row r="15" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="126"/>
       <c r="B15" s="126"/>
       <c r="C15" s="127"/>
@@ -4489,7 +4489,7 @@
       <c r="R15" s="127"/>
       <c r="S15" s="131"/>
     </row>
-    <row r="16" spans="1:19" s="128" customFormat="1">
+    <row r="16" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A16" s="126"/>
       <c r="B16" s="126"/>
       <c r="C16" s="127"/>
@@ -4510,7 +4510,7 @@
       <c r="R16" s="127"/>
       <c r="S16" s="131"/>
     </row>
-    <row r="17" spans="1:19" s="128" customFormat="1">
+    <row r="17" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A17" s="126"/>
       <c r="B17" s="126"/>
       <c r="C17" s="127"/>
@@ -4531,7 +4531,7 @@
       <c r="R17" s="127"/>
       <c r="S17" s="131"/>
     </row>
-    <row r="18" spans="1:19" s="128" customFormat="1">
+    <row r="18" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A18" s="126"/>
       <c r="B18" s="126"/>
       <c r="C18" s="127"/>
@@ -4552,7 +4552,7 @@
       <c r="R18" s="127"/>
       <c r="S18" s="131"/>
     </row>
-    <row r="19" spans="1:19" s="128" customFormat="1">
+    <row r="19" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A19" s="126"/>
       <c r="B19" s="126"/>
       <c r="C19" s="127"/>
@@ -4573,7 +4573,7 @@
       <c r="R19" s="127"/>
       <c r="S19" s="131"/>
     </row>
-    <row r="20" spans="1:19" s="128" customFormat="1">
+    <row r="20" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A20" s="126"/>
       <c r="B20" s="126"/>
       <c r="C20" s="127"/>
@@ -4594,7 +4594,7 @@
       <c r="R20" s="127"/>
       <c r="S20" s="131"/>
     </row>
-    <row r="21" spans="1:19" s="128" customFormat="1">
+    <row r="21" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A21" s="126"/>
       <c r="B21" s="126"/>
       <c r="C21" s="127"/>
@@ -4615,7 +4615,7 @@
       <c r="R21" s="127"/>
       <c r="S21" s="131"/>
     </row>
-    <row r="22" spans="1:19" s="128" customFormat="1">
+    <row r="22" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A22" s="126"/>
       <c r="B22" s="126"/>
       <c r="C22" s="127"/>
@@ -4636,7 +4636,7 @@
       <c r="R22" s="127"/>
       <c r="S22" s="131"/>
     </row>
-    <row r="23" spans="1:19" s="128" customFormat="1">
+    <row r="23" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A23" s="126"/>
       <c r="B23" s="126"/>
       <c r="C23" s="127"/>
@@ -4657,7 +4657,7 @@
       <c r="R23" s="127"/>
       <c r="S23" s="131"/>
     </row>
-    <row r="24" spans="1:19" s="128" customFormat="1">
+    <row r="24" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A24" s="126"/>
       <c r="B24" s="126"/>
       <c r="C24" s="127"/>
@@ -4678,7 +4678,7 @@
       <c r="R24" s="127"/>
       <c r="S24" s="131"/>
     </row>
-    <row r="25" spans="1:19" s="128" customFormat="1">
+    <row r="25" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A25" s="126"/>
       <c r="B25" s="126"/>
       <c r="C25" s="127"/>
@@ -4699,7 +4699,7 @@
       <c r="R25" s="127"/>
       <c r="S25" s="131"/>
     </row>
-    <row r="26" spans="1:19" s="128" customFormat="1">
+    <row r="26" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A26" s="126"/>
       <c r="B26" s="126"/>
       <c r="C26" s="127"/>
@@ -4720,7 +4720,7 @@
       <c r="R26" s="127"/>
       <c r="S26" s="131"/>
     </row>
-    <row r="27" spans="1:19" s="128" customFormat="1">
+    <row r="27" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A27" s="126"/>
       <c r="B27" s="126"/>
       <c r="C27" s="127"/>
@@ -4741,7 +4741,7 @@
       <c r="R27" s="127"/>
       <c r="S27" s="131"/>
     </row>
-    <row r="28" spans="1:19" s="128" customFormat="1">
+    <row r="28" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A28" s="126"/>
       <c r="B28" s="126"/>
       <c r="C28" s="127"/>
@@ -4762,7 +4762,7 @@
       <c r="R28" s="127"/>
       <c r="S28" s="131"/>
     </row>
-    <row r="29" spans="1:19" s="128" customFormat="1">
+    <row r="29" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A29" s="126"/>
       <c r="B29" s="126"/>
       <c r="C29" s="127"/>
@@ -4783,7 +4783,7 @@
       <c r="R29" s="127"/>
       <c r="S29" s="131"/>
     </row>
-    <row r="30" spans="1:19" s="128" customFormat="1">
+    <row r="30" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A30" s="129"/>
       <c r="B30" s="129"/>
       <c r="D30" s="131"/>
@@ -4803,7 +4803,7 @@
       <c r="R30" s="127"/>
       <c r="S30" s="131"/>
     </row>
-    <row r="31" spans="1:19" s="128" customFormat="1">
+    <row r="31" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A31" s="129"/>
       <c r="B31" s="129"/>
       <c r="D31" s="131"/>
@@ -4823,7 +4823,7 @@
       <c r="R31" s="127"/>
       <c r="S31" s="131"/>
     </row>
-    <row r="32" spans="1:19" s="128" customFormat="1">
+    <row r="32" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A32" s="129"/>
       <c r="B32" s="129"/>
       <c r="D32" s="131"/>
@@ -4843,7 +4843,7 @@
       <c r="R32" s="127"/>
       <c r="S32" s="131"/>
     </row>
-    <row r="33" spans="1:19" s="128" customFormat="1">
+    <row r="33" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A33" s="129"/>
       <c r="B33" s="129"/>
       <c r="D33" s="131"/>
@@ -4863,7 +4863,7 @@
       <c r="R33" s="127"/>
       <c r="S33" s="131"/>
     </row>
-    <row r="34" spans="1:19" s="128" customFormat="1">
+    <row r="34" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A34" s="129"/>
       <c r="B34" s="129"/>
       <c r="D34" s="131"/>
@@ -4883,7 +4883,7 @@
       <c r="R34" s="127"/>
       <c r="S34" s="131"/>
     </row>
-    <row r="35" spans="1:19" s="128" customFormat="1">
+    <row r="35" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A35" s="129"/>
       <c r="B35" s="129"/>
       <c r="D35" s="131"/>
@@ -4903,7 +4903,7 @@
       <c r="R35" s="127"/>
       <c r="S35" s="131"/>
     </row>
-    <row r="36" spans="1:19" s="128" customFormat="1">
+    <row r="36" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A36" s="129"/>
       <c r="B36" s="129"/>
       <c r="D36" s="131"/>
@@ -4923,7 +4923,7 @@
       <c r="R36" s="127"/>
       <c r="S36" s="131"/>
     </row>
-    <row r="37" spans="1:19" s="128" customFormat="1">
+    <row r="37" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A37" s="129"/>
       <c r="B37" s="129"/>
       <c r="D37" s="131"/>
@@ -4943,7 +4943,7 @@
       <c r="R37" s="127"/>
       <c r="S37" s="131"/>
     </row>
-    <row r="38" spans="1:19" s="128" customFormat="1">
+    <row r="38" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A38" s="129"/>
       <c r="B38" s="129"/>
       <c r="D38" s="131"/>
@@ -4962,7 +4962,7 @@
       <c r="Q38" s="129"/>
       <c r="S38" s="131"/>
     </row>
-    <row r="39" spans="1:19" s="128" customFormat="1">
+    <row r="39" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A39" s="129"/>
       <c r="B39" s="129"/>
       <c r="D39" s="131"/>
@@ -4981,7 +4981,7 @@
       <c r="Q39" s="129"/>
       <c r="S39" s="131"/>
     </row>
-    <row r="40" spans="1:19" s="128" customFormat="1">
+    <row r="40" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A40" s="129"/>
       <c r="B40" s="129"/>
       <c r="D40" s="131"/>
@@ -5000,7 +5000,7 @@
       <c r="Q40" s="129"/>
       <c r="S40" s="131"/>
     </row>
-    <row r="41" spans="1:19" s="128" customFormat="1">
+    <row r="41" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A41" s="129"/>
       <c r="B41" s="129"/>
       <c r="D41" s="131"/>
@@ -5018,7 +5018,7 @@
       <c r="Q41" s="129"/>
       <c r="S41" s="131"/>
     </row>
-    <row r="42" spans="1:19" s="128" customFormat="1">
+    <row r="42" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A42" s="129"/>
       <c r="B42" s="129"/>
       <c r="D42" s="131"/>
@@ -5036,7 +5036,7 @@
       <c r="Q42" s="129"/>
       <c r="S42" s="131"/>
     </row>
-    <row r="43" spans="1:19" s="128" customFormat="1">
+    <row r="43" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A43" s="129"/>
       <c r="B43" s="129"/>
       <c r="D43" s="131"/>
@@ -5054,7 +5054,7 @@
       <c r="Q43" s="129"/>
       <c r="S43" s="131"/>
     </row>
-    <row r="44" spans="1:19" s="128" customFormat="1">
+    <row r="44" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A44" s="129"/>
       <c r="B44" s="129"/>
       <c r="D44" s="131"/>
@@ -5072,7 +5072,7 @@
       <c r="Q44" s="129"/>
       <c r="S44" s="131"/>
     </row>
-    <row r="45" spans="1:19" s="128" customFormat="1">
+    <row r="45" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A45" s="129"/>
       <c r="B45" s="129"/>
       <c r="D45" s="131"/>
@@ -5090,7 +5090,7 @@
       <c r="Q45" s="129"/>
       <c r="S45" s="131"/>
     </row>
-    <row r="46" spans="1:19" s="128" customFormat="1">
+    <row r="46" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A46" s="129"/>
       <c r="B46" s="129"/>
       <c r="D46" s="131"/>
@@ -5108,7 +5108,7 @@
       <c r="Q46" s="129"/>
       <c r="S46" s="131"/>
     </row>
-    <row r="47" spans="1:19" s="128" customFormat="1">
+    <row r="47" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A47" s="129"/>
       <c r="B47" s="129"/>
       <c r="D47" s="131"/>
@@ -5126,7 +5126,7 @@
       <c r="Q47" s="129"/>
       <c r="S47" s="131"/>
     </row>
-    <row r="48" spans="1:19" s="128" customFormat="1">
+    <row r="48" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A48" s="129"/>
       <c r="B48" s="129"/>
       <c r="D48" s="131"/>
@@ -5144,7 +5144,7 @@
       <c r="Q48" s="129"/>
       <c r="S48" s="131"/>
     </row>
-    <row r="49" spans="1:19" s="128" customFormat="1">
+    <row r="49" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A49" s="129"/>
       <c r="B49" s="129"/>
       <c r="D49" s="131"/>
@@ -5162,7 +5162,7 @@
       <c r="Q49" s="129"/>
       <c r="S49" s="131"/>
     </row>
-    <row r="50" spans="1:19" s="128" customFormat="1">
+    <row r="50" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A50" s="129"/>
       <c r="B50" s="129"/>
       <c r="D50" s="131"/>
@@ -5180,7 +5180,7 @@
       <c r="Q50" s="129"/>
       <c r="S50" s="131"/>
     </row>
-    <row r="51" spans="1:19" s="128" customFormat="1">
+    <row r="51" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A51" s="129"/>
       <c r="B51" s="129"/>
       <c r="D51" s="131"/>
@@ -5198,7 +5198,7 @@
       <c r="Q51" s="129"/>
       <c r="S51" s="131"/>
     </row>
-    <row r="52" spans="1:19" s="128" customFormat="1">
+    <row r="52" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A52" s="129"/>
       <c r="B52" s="129"/>
       <c r="D52" s="131"/>
@@ -5216,7 +5216,7 @@
       <c r="Q52" s="129"/>
       <c r="S52" s="131"/>
     </row>
-    <row r="53" spans="1:19" s="128" customFormat="1">
+    <row r="53" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A53" s="129"/>
       <c r="B53" s="129"/>
       <c r="D53" s="131"/>
@@ -5234,7 +5234,7 @@
       <c r="Q53" s="129"/>
       <c r="S53" s="131"/>
     </row>
-    <row r="54" spans="1:19" s="128" customFormat="1">
+    <row r="54" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A54" s="129"/>
       <c r="B54" s="129"/>
       <c r="D54" s="131"/>
@@ -5252,7 +5252,7 @@
       <c r="Q54" s="129"/>
       <c r="S54" s="131"/>
     </row>
-    <row r="55" spans="1:19" s="128" customFormat="1">
+    <row r="55" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A55" s="129"/>
       <c r="B55" s="129"/>
       <c r="D55" s="131"/>
@@ -5270,7 +5270,7 @@
       <c r="Q55" s="129"/>
       <c r="S55" s="131"/>
     </row>
-    <row r="56" spans="1:19" s="128" customFormat="1">
+    <row r="56" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A56" s="129"/>
       <c r="B56" s="129"/>
       <c r="D56" s="131"/>
@@ -5288,7 +5288,7 @@
       <c r="Q56" s="129"/>
       <c r="S56" s="131"/>
     </row>
-    <row r="57" spans="1:19" s="128" customFormat="1">
+    <row r="57" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A57" s="129"/>
       <c r="B57" s="129"/>
       <c r="D57" s="131"/>
@@ -5306,7 +5306,7 @@
       <c r="Q57" s="129"/>
       <c r="S57" s="131"/>
     </row>
-    <row r="58" spans="1:19" s="128" customFormat="1">
+    <row r="58" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A58" s="129"/>
       <c r="B58" s="129"/>
       <c r="D58" s="131"/>
@@ -5324,7 +5324,7 @@
       <c r="Q58" s="129"/>
       <c r="S58" s="131"/>
     </row>
-    <row r="59" spans="1:19" s="128" customFormat="1">
+    <row r="59" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A59" s="129"/>
       <c r="B59" s="129"/>
       <c r="D59" s="131"/>
@@ -5342,7 +5342,7 @@
       <c r="Q59" s="129"/>
       <c r="S59" s="131"/>
     </row>
-    <row r="60" spans="1:19" s="128" customFormat="1">
+    <row r="60" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A60" s="129"/>
       <c r="B60" s="129"/>
       <c r="D60" s="131"/>
@@ -5360,7 +5360,7 @@
       <c r="Q60" s="129"/>
       <c r="S60" s="131"/>
     </row>
-    <row r="61" spans="1:19" s="128" customFormat="1">
+    <row r="61" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A61" s="129"/>
       <c r="B61" s="129"/>
       <c r="D61" s="131"/>
@@ -5378,7 +5378,7 @@
       <c r="Q61" s="129"/>
       <c r="S61" s="131"/>
     </row>
-    <row r="62" spans="1:19" s="128" customFormat="1">
+    <row r="62" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A62" s="129"/>
       <c r="B62" s="129"/>
       <c r="D62" s="131"/>
@@ -5396,7 +5396,7 @@
       <c r="Q62" s="129"/>
       <c r="S62" s="131"/>
     </row>
-    <row r="63" spans="1:19" s="128" customFormat="1">
+    <row r="63" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A63" s="129"/>
       <c r="B63" s="129"/>
       <c r="D63" s="131"/>
@@ -5414,7 +5414,7 @@
       <c r="Q63" s="129"/>
       <c r="S63" s="131"/>
     </row>
-    <row r="64" spans="1:19" s="128" customFormat="1">
+    <row r="64" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A64" s="129"/>
       <c r="B64" s="129"/>
       <c r="D64" s="131"/>
@@ -5432,7 +5432,7 @@
       <c r="Q64" s="129"/>
       <c r="S64" s="131"/>
     </row>
-    <row r="65" spans="1:19" s="128" customFormat="1">
+    <row r="65" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A65" s="129"/>
       <c r="B65" s="129"/>
       <c r="D65" s="131"/>
@@ -5450,7 +5450,7 @@
       <c r="Q65" s="129"/>
       <c r="S65" s="131"/>
     </row>
-    <row r="66" spans="1:19" s="128" customFormat="1">
+    <row r="66" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A66" s="129"/>
       <c r="B66" s="129"/>
       <c r="D66" s="131"/>
@@ -5468,7 +5468,7 @@
       <c r="Q66" s="129"/>
       <c r="S66" s="131"/>
     </row>
-    <row r="67" spans="1:19" s="128" customFormat="1">
+    <row r="67" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A67" s="129"/>
       <c r="B67" s="129"/>
       <c r="D67" s="131"/>
@@ -5486,7 +5486,7 @@
       <c r="Q67" s="129"/>
       <c r="S67" s="131"/>
     </row>
-    <row r="68" spans="1:19" s="128" customFormat="1">
+    <row r="68" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A68" s="129"/>
       <c r="B68" s="129"/>
       <c r="D68" s="131"/>
@@ -5504,7 +5504,7 @@
       <c r="Q68" s="129"/>
       <c r="S68" s="131"/>
     </row>
-    <row r="69" spans="1:19" s="128" customFormat="1">
+    <row r="69" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A69" s="129"/>
       <c r="B69" s="129"/>
       <c r="D69" s="131"/>
@@ -5522,7 +5522,7 @@
       <c r="Q69" s="129"/>
       <c r="S69" s="131"/>
     </row>
-    <row r="70" spans="1:19" s="128" customFormat="1">
+    <row r="70" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A70" s="129"/>
       <c r="B70" s="129"/>
       <c r="D70" s="131"/>
@@ -5539,7 +5539,7 @@
       <c r="Q70" s="129"/>
       <c r="S70" s="131"/>
     </row>
-    <row r="71" spans="1:19" s="128" customFormat="1">
+    <row r="71" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A71" s="129"/>
       <c r="B71" s="129"/>
       <c r="D71" s="131"/>
@@ -5556,7 +5556,7 @@
       <c r="Q71" s="129"/>
       <c r="S71" s="131"/>
     </row>
-    <row r="72" spans="1:19" s="128" customFormat="1">
+    <row r="72" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A72" s="129"/>
       <c r="B72" s="129"/>
       <c r="D72" s="131"/>
@@ -5573,7 +5573,7 @@
       <c r="Q72" s="129"/>
       <c r="S72" s="131"/>
     </row>
-    <row r="73" spans="1:19" s="128" customFormat="1">
+    <row r="73" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A73" s="129"/>
       <c r="B73" s="129"/>
       <c r="D73" s="131"/>
@@ -5590,7 +5590,7 @@
       <c r="Q73" s="129"/>
       <c r="S73" s="131"/>
     </row>
-    <row r="74" spans="1:19" s="128" customFormat="1">
+    <row r="74" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A74" s="129"/>
       <c r="B74" s="129"/>
       <c r="D74" s="131"/>
@@ -5607,7 +5607,7 @@
       <c r="Q74" s="129"/>
       <c r="S74" s="131"/>
     </row>
-    <row r="75" spans="1:19" s="128" customFormat="1">
+    <row r="75" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A75" s="129"/>
       <c r="B75" s="129"/>
       <c r="D75" s="131"/>
@@ -5624,7 +5624,7 @@
       <c r="Q75" s="129"/>
       <c r="S75" s="131"/>
     </row>
-    <row r="76" spans="1:19" s="128" customFormat="1">
+    <row r="76" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A76" s="129"/>
       <c r="B76" s="129"/>
       <c r="D76" s="131"/>
@@ -5641,7 +5641,7 @@
       <c r="Q76" s="129"/>
       <c r="S76" s="131"/>
     </row>
-    <row r="77" spans="1:19" s="128" customFormat="1">
+    <row r="77" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A77" s="129"/>
       <c r="B77" s="129"/>
       <c r="D77" s="131"/>
@@ -5658,7 +5658,7 @@
       <c r="Q77" s="129"/>
       <c r="S77" s="131"/>
     </row>
-    <row r="78" spans="1:19" s="128" customFormat="1">
+    <row r="78" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A78" s="129"/>
       <c r="B78" s="129"/>
       <c r="D78" s="131"/>
@@ -5675,7 +5675,7 @@
       <c r="Q78" s="129"/>
       <c r="S78" s="131"/>
     </row>
-    <row r="79" spans="1:19" s="128" customFormat="1">
+    <row r="79" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A79" s="129"/>
       <c r="B79" s="129"/>
       <c r="D79" s="131"/>
@@ -5692,7 +5692,7 @@
       <c r="Q79" s="129"/>
       <c r="S79" s="131"/>
     </row>
-    <row r="80" spans="1:19" s="128" customFormat="1">
+    <row r="80" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A80" s="129"/>
       <c r="B80" s="129"/>
       <c r="D80" s="131"/>
@@ -5709,7 +5709,7 @@
       <c r="Q80" s="129"/>
       <c r="S80" s="131"/>
     </row>
-    <row r="81" spans="1:19" s="128" customFormat="1">
+    <row r="81" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A81" s="129"/>
       <c r="B81" s="129"/>
       <c r="D81" s="131"/>
@@ -5726,7 +5726,7 @@
       <c r="Q81" s="129"/>
       <c r="S81" s="131"/>
     </row>
-    <row r="82" spans="1:19" s="128" customFormat="1">
+    <row r="82" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A82" s="129"/>
       <c r="B82" s="129"/>
       <c r="D82" s="131"/>
@@ -5743,7 +5743,7 @@
       <c r="Q82" s="129"/>
       <c r="S82" s="131"/>
     </row>
-    <row r="83" spans="1:19" s="128" customFormat="1">
+    <row r="83" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A83" s="129"/>
       <c r="B83" s="129"/>
       <c r="D83" s="131"/>
@@ -5760,7 +5760,7 @@
       <c r="Q83" s="129"/>
       <c r="S83" s="131"/>
     </row>
-    <row r="84" spans="1:19" s="128" customFormat="1">
+    <row r="84" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A84" s="129"/>
       <c r="B84" s="129"/>
       <c r="D84" s="131"/>
@@ -5777,7 +5777,7 @@
       <c r="Q84" s="129"/>
       <c r="S84" s="131"/>
     </row>
-    <row r="85" spans="1:19" s="128" customFormat="1">
+    <row r="85" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A85" s="129"/>
       <c r="B85" s="129"/>
       <c r="D85" s="131"/>
@@ -5794,7 +5794,7 @@
       <c r="Q85" s="129"/>
       <c r="S85" s="131"/>
     </row>
-    <row r="86" spans="1:19" s="128" customFormat="1">
+    <row r="86" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A86" s="129"/>
       <c r="B86" s="129"/>
       <c r="D86" s="131"/>
@@ -5811,7 +5811,7 @@
       <c r="Q86" s="129"/>
       <c r="S86" s="131"/>
     </row>
-    <row r="87" spans="1:19" s="128" customFormat="1">
+    <row r="87" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A87" s="129"/>
       <c r="B87" s="129"/>
       <c r="D87" s="131"/>
@@ -5828,7 +5828,7 @@
       <c r="Q87" s="129"/>
       <c r="S87" s="131"/>
     </row>
-    <row r="88" spans="1:19" s="128" customFormat="1">
+    <row r="88" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A88" s="129"/>
       <c r="B88" s="129"/>
       <c r="D88" s="131"/>
@@ -5845,7 +5845,7 @@
       <c r="Q88" s="129"/>
       <c r="S88" s="131"/>
     </row>
-    <row r="89" spans="1:19" s="128" customFormat="1">
+    <row r="89" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A89" s="129"/>
       <c r="B89" s="129"/>
       <c r="D89" s="131"/>
@@ -5862,7 +5862,7 @@
       <c r="Q89" s="129"/>
       <c r="S89" s="131"/>
     </row>
-    <row r="90" spans="1:19" s="128" customFormat="1">
+    <row r="90" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A90" s="129"/>
       <c r="B90" s="129"/>
       <c r="D90" s="131"/>
@@ -5879,7 +5879,7 @@
       <c r="Q90" s="129"/>
       <c r="S90" s="131"/>
     </row>
-    <row r="91" spans="1:19" s="128" customFormat="1">
+    <row r="91" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A91" s="129"/>
       <c r="B91" s="129"/>
       <c r="D91" s="131"/>
@@ -5896,7 +5896,7 @@
       <c r="Q91" s="129"/>
       <c r="S91" s="131"/>
     </row>
-    <row r="92" spans="1:19" s="128" customFormat="1">
+    <row r="92" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A92" s="129"/>
       <c r="B92" s="129"/>
       <c r="D92" s="131"/>
@@ -5913,7 +5913,7 @@
       <c r="Q92" s="129"/>
       <c r="S92" s="131"/>
     </row>
-    <row r="93" spans="1:19" s="128" customFormat="1">
+    <row r="93" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A93" s="129"/>
       <c r="B93" s="129"/>
       <c r="D93" s="131"/>
@@ -5930,7 +5930,7 @@
       <c r="Q93" s="129"/>
       <c r="S93" s="131"/>
     </row>
-    <row r="94" spans="1:19" s="128" customFormat="1">
+    <row r="94" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A94" s="129"/>
       <c r="B94" s="129"/>
       <c r="D94" s="131"/>
@@ -5947,7 +5947,7 @@
       <c r="Q94" s="129"/>
       <c r="S94" s="131"/>
     </row>
-    <row r="95" spans="1:19" s="128" customFormat="1">
+    <row r="95" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A95" s="129"/>
       <c r="B95" s="129"/>
       <c r="D95" s="131"/>
@@ -5964,7 +5964,7 @@
       <c r="Q95" s="129"/>
       <c r="S95" s="131"/>
     </row>
-    <row r="96" spans="1:19" s="128" customFormat="1">
+    <row r="96" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A96" s="129"/>
       <c r="B96" s="129"/>
       <c r="D96" s="131"/>
@@ -5981,7 +5981,7 @@
       <c r="Q96" s="129"/>
       <c r="S96" s="131"/>
     </row>
-    <row r="97" spans="1:19" s="128" customFormat="1">
+    <row r="97" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A97" s="129"/>
       <c r="B97" s="129"/>
       <c r="D97" s="131"/>
@@ -5998,7 +5998,7 @@
       <c r="Q97" s="129"/>
       <c r="S97" s="131"/>
     </row>
-    <row r="98" spans="1:19" s="128" customFormat="1">
+    <row r="98" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A98" s="129"/>
       <c r="B98" s="129"/>
       <c r="D98" s="131"/>
@@ -6015,7 +6015,7 @@
       <c r="Q98" s="129"/>
       <c r="S98" s="131"/>
     </row>
-    <row r="99" spans="1:19" s="128" customFormat="1">
+    <row r="99" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A99" s="129"/>
       <c r="B99" s="129"/>
       <c r="D99" s="131"/>
@@ -6032,7 +6032,7 @@
       <c r="Q99" s="129"/>
       <c r="S99" s="131"/>
     </row>
-    <row r="100" spans="1:19" s="128" customFormat="1">
+    <row r="100" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A100" s="129"/>
       <c r="B100" s="129"/>
       <c r="D100" s="131"/>
@@ -6049,7 +6049,7 @@
       <c r="Q100" s="129"/>
       <c r="S100" s="131"/>
     </row>
-    <row r="101" spans="1:19" s="128" customFormat="1">
+    <row r="101" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A101" s="129"/>
       <c r="B101" s="129"/>
       <c r="D101" s="131"/>
@@ -6066,7 +6066,7 @@
       <c r="Q101" s="129"/>
       <c r="S101" s="131"/>
     </row>
-    <row r="102" spans="1:19" s="128" customFormat="1">
+    <row r="102" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A102" s="129"/>
       <c r="B102" s="129"/>
       <c r="D102" s="131"/>
@@ -6083,7 +6083,7 @@
       <c r="Q102" s="129"/>
       <c r="S102" s="131"/>
     </row>
-    <row r="103" spans="1:19" s="128" customFormat="1">
+    <row r="103" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A103" s="129"/>
       <c r="B103" s="129"/>
       <c r="D103" s="131"/>
@@ -6100,7 +6100,7 @@
       <c r="Q103" s="129"/>
       <c r="S103" s="131"/>
     </row>
-    <row r="104" spans="1:19" s="128" customFormat="1">
+    <row r="104" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A104" s="129"/>
       <c r="B104" s="129"/>
       <c r="D104" s="131"/>
@@ -6117,7 +6117,7 @@
       <c r="Q104" s="129"/>
       <c r="S104" s="131"/>
     </row>
-    <row r="105" spans="1:19" s="128" customFormat="1">
+    <row r="105" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A105" s="129"/>
       <c r="B105" s="129"/>
       <c r="D105" s="131"/>
@@ -6134,7 +6134,7 @@
       <c r="Q105" s="129"/>
       <c r="S105" s="131"/>
     </row>
-    <row r="106" spans="1:19" s="128" customFormat="1">
+    <row r="106" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A106" s="129"/>
       <c r="B106" s="129"/>
       <c r="D106" s="131"/>
@@ -6151,7 +6151,7 @@
       <c r="Q106" s="129"/>
       <c r="S106" s="131"/>
     </row>
-    <row r="107" spans="1:19" s="128" customFormat="1">
+    <row r="107" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A107" s="129"/>
       <c r="B107" s="129"/>
       <c r="D107" s="131"/>
@@ -6168,7 +6168,7 @@
       <c r="Q107" s="129"/>
       <c r="S107" s="131"/>
     </row>
-    <row r="108" spans="1:19" s="128" customFormat="1">
+    <row r="108" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A108" s="129"/>
       <c r="B108" s="129"/>
       <c r="D108" s="131"/>
@@ -6185,7 +6185,7 @@
       <c r="Q108" s="129"/>
       <c r="S108" s="131"/>
     </row>
-    <row r="109" spans="1:19" s="128" customFormat="1">
+    <row r="109" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A109" s="129"/>
       <c r="B109" s="129"/>
       <c r="D109" s="131"/>
@@ -6202,7 +6202,7 @@
       <c r="Q109" s="129"/>
       <c r="S109" s="131"/>
     </row>
-    <row r="110" spans="1:19" s="128" customFormat="1">
+    <row r="110" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A110" s="129"/>
       <c r="B110" s="129"/>
       <c r="D110" s="131"/>
@@ -6219,7 +6219,7 @@
       <c r="Q110" s="129"/>
       <c r="S110" s="131"/>
     </row>
-    <row r="111" spans="1:19" s="128" customFormat="1">
+    <row r="111" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A111" s="129"/>
       <c r="B111" s="129"/>
       <c r="D111" s="131"/>
@@ -6236,7 +6236,7 @@
       <c r="Q111" s="129"/>
       <c r="S111" s="131"/>
     </row>
-    <row r="112" spans="1:19" s="128" customFormat="1">
+    <row r="112" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A112" s="129"/>
       <c r="B112" s="129"/>
       <c r="D112" s="131"/>
@@ -6253,7 +6253,7 @@
       <c r="Q112" s="129"/>
       <c r="S112" s="131"/>
     </row>
-    <row r="113" spans="1:19" s="128" customFormat="1">
+    <row r="113" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A113" s="129"/>
       <c r="B113" s="129"/>
       <c r="D113" s="131"/>
@@ -6270,7 +6270,7 @@
       <c r="Q113" s="129"/>
       <c r="S113" s="131"/>
     </row>
-    <row r="114" spans="1:19" s="128" customFormat="1">
+    <row r="114" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A114" s="129"/>
       <c r="B114" s="129"/>
       <c r="D114" s="131"/>
@@ -6287,7 +6287,7 @@
       <c r="Q114" s="129"/>
       <c r="S114" s="131"/>
     </row>
-    <row r="115" spans="1:19" s="128" customFormat="1">
+    <row r="115" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A115" s="129"/>
       <c r="B115" s="129"/>
       <c r="D115" s="131"/>
@@ -6304,7 +6304,7 @@
       <c r="Q115" s="129"/>
       <c r="S115" s="131"/>
     </row>
-    <row r="116" spans="1:19" s="128" customFormat="1">
+    <row r="116" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A116" s="129"/>
       <c r="B116" s="129"/>
       <c r="D116" s="131"/>
@@ -6321,7 +6321,7 @@
       <c r="Q116" s="129"/>
       <c r="S116" s="131"/>
     </row>
-    <row r="117" spans="1:19" s="128" customFormat="1">
+    <row r="117" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A117" s="129"/>
       <c r="B117" s="129"/>
       <c r="D117" s="131"/>
@@ -6338,7 +6338,7 @@
       <c r="Q117" s="129"/>
       <c r="S117" s="131"/>
     </row>
-    <row r="118" spans="1:19" s="128" customFormat="1">
+    <row r="118" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A118" s="129"/>
       <c r="B118" s="129"/>
       <c r="D118" s="131"/>
@@ -6355,7 +6355,7 @@
       <c r="Q118" s="129"/>
       <c r="S118" s="131"/>
     </row>
-    <row r="119" spans="1:19" s="128" customFormat="1">
+    <row r="119" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A119" s="129"/>
       <c r="B119" s="129"/>
       <c r="D119" s="131"/>
@@ -6372,7 +6372,7 @@
       <c r="Q119" s="129"/>
       <c r="S119" s="131"/>
     </row>
-    <row r="120" spans="1:19" s="128" customFormat="1">
+    <row r="120" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A120" s="129"/>
       <c r="B120" s="129"/>
       <c r="D120" s="131"/>
@@ -6389,7 +6389,7 @@
       <c r="Q120" s="129"/>
       <c r="S120" s="131"/>
     </row>
-    <row r="121" spans="1:19" s="128" customFormat="1">
+    <row r="121" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A121" s="129"/>
       <c r="B121" s="129"/>
       <c r="D121" s="131"/>
@@ -6406,7 +6406,7 @@
       <c r="Q121" s="129"/>
       <c r="S121" s="131"/>
     </row>
-    <row r="122" spans="1:19" s="128" customFormat="1">
+    <row r="122" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A122" s="129"/>
       <c r="B122" s="129"/>
       <c r="D122" s="131"/>
@@ -6423,7 +6423,7 @@
       <c r="Q122" s="129"/>
       <c r="S122" s="131"/>
     </row>
-    <row r="123" spans="1:19" s="128" customFormat="1">
+    <row r="123" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A123" s="129"/>
       <c r="B123" s="129"/>
       <c r="D123" s="131"/>
@@ -6440,7 +6440,7 @@
       <c r="Q123" s="129"/>
       <c r="S123" s="131"/>
     </row>
-    <row r="124" spans="1:19" s="128" customFormat="1">
+    <row r="124" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A124" s="129"/>
       <c r="B124" s="129"/>
       <c r="D124" s="131"/>
@@ -6457,7 +6457,7 @@
       <c r="Q124" s="129"/>
       <c r="S124" s="131"/>
     </row>
-    <row r="125" spans="1:19" s="128" customFormat="1">
+    <row r="125" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A125" s="129"/>
       <c r="B125" s="129"/>
       <c r="D125" s="131"/>
@@ -6474,7 +6474,7 @@
       <c r="Q125" s="129"/>
       <c r="S125" s="131"/>
     </row>
-    <row r="126" spans="1:19" s="128" customFormat="1">
+    <row r="126" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A126" s="129"/>
       <c r="B126" s="129"/>
       <c r="D126" s="131"/>
@@ -6491,7 +6491,7 @@
       <c r="Q126" s="129"/>
       <c r="S126" s="131"/>
     </row>
-    <row r="127" spans="1:19" s="128" customFormat="1">
+    <row r="127" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A127" s="129"/>
       <c r="B127" s="129"/>
       <c r="D127" s="131"/>
@@ -6508,7 +6508,7 @@
       <c r="Q127" s="129"/>
       <c r="S127" s="131"/>
     </row>
-    <row r="128" spans="1:19" s="128" customFormat="1">
+    <row r="128" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A128" s="129"/>
       <c r="B128" s="129"/>
       <c r="D128" s="131"/>
@@ -6525,7 +6525,7 @@
       <c r="Q128" s="129"/>
       <c r="S128" s="131"/>
     </row>
-    <row r="129" spans="1:19" s="128" customFormat="1">
+    <row r="129" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A129" s="129"/>
       <c r="B129" s="129"/>
       <c r="D129" s="131"/>
@@ -6542,7 +6542,7 @@
       <c r="Q129" s="129"/>
       <c r="S129" s="131"/>
     </row>
-    <row r="130" spans="1:19" s="128" customFormat="1">
+    <row r="130" spans="1:19" s="128" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A130" s="129"/>
       <c r="B130" s="129"/>
       <c r="D130" s="131"/>
@@ -6568,11 +6568,6 @@
     <protectedRange sqref="A11:D100" name="Phase 1"/>
   </protectedRanges>
   <mergeCells count="12">
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K8:N8"/>
     <mergeCell ref="P4:S4"/>
     <mergeCell ref="P7:S7"/>
     <mergeCell ref="P8:S8"/>
@@ -6580,12 +6575,26 @@
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="F7:I7"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100234C71A0D07BF2478619420DEE8E169E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="99bb204b3d07a6ecd74fb57cbeaa66e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ab021141-f644-459a-a154-005270a80161" xmlns:ns3="71e8357a-e36d-4581-945d-62ca331a1321" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d58c8454a3da09c8f35be92b754e7ad9" ns2:_="" ns3:_="">
     <xsd:import namespace="ab021141-f644-459a-a154-005270a80161"/>
@@ -6814,15 +6823,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6842,15 +6842,41 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFE325BB-B2FC-477D-B11E-B50398C86E78}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F0DEB1B-B56C-4659-9DDA-D3892EDC5BCB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F0DEB1B-B56C-4659-9DDA-D3892EDC5BCB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFE325BB-B2FC-477D-B11E-B50398C86E78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ab021141-f644-459a-a154-005270a80161"/>
+    <ds:schemaRef ds:uri="71e8357a-e36d-4581-945d-62ca331a1321"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11BE4EBD-D9EA-49BC-A9FF-A36BFBB89169}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11BE4EBD-D9EA-49BC-A9FF-A36BFBB89169}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71e8357a-e36d-4581-945d-62ca331a1321"/>
+    <ds:schemaRef ds:uri="ab021141-f644-459a-a154-005270a80161"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>